<commit_message>
Update webpage data 20200710
</commit_message>
<xml_diff>
--- a/outputgap.xlsx
+++ b/outputgap.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="outputgap" localSheetId="0">Tabelle1!$A$1:$C$214</definedName>
+    <definedName name="outputgap_1" localSheetId="0">Tabelle1!$A$1:$B$214</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +29,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="outputgap" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="850" sourceFile="C:\Users\tweak\Desktop\outputgapnow.github.io\outputgap.csv" decimal="," thousands="." tab="0" semicolon="1">
+    <textPr codePage="850" sourceFile="C:\Users\tweak\Desktop\outputgapnow.github.io\outputgap.csv" decimal="," thousands="." semicolon="1">
       <textFields count="3">
         <textField/>
         <textField/>
@@ -102,7 +102,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="outputgap" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="outputgap_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -368,2366 +368,1728 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C214"/>
+  <dimension ref="A1:B214"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0</v>
+        <v>1967.25</v>
       </c>
       <c r="B2">
-        <v>1967.25</v>
-      </c>
-      <c r="C2">
         <v>3.1217449205119299</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
+        <v>1967.5</v>
       </c>
       <c r="B3">
-        <v>1967.5</v>
-      </c>
-      <c r="C3">
         <v>3.66577993668681</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2</v>
+        <v>1967.75</v>
       </c>
       <c r="B4">
-        <v>1967.75</v>
-      </c>
-      <c r="C4">
         <v>3.59515546639506</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3</v>
+        <v>1968</v>
       </c>
       <c r="B5">
-        <v>1968</v>
-      </c>
-      <c r="C5">
         <v>3.9271466382095799</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>4</v>
+        <v>1968.25</v>
       </c>
       <c r="B6">
-        <v>1968.25</v>
-      </c>
-      <c r="C6">
         <v>4.3216774356072696</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>5</v>
+        <v>1968.5</v>
       </c>
       <c r="B7">
-        <v>1968.5</v>
-      </c>
-      <c r="C7">
         <v>4.5025162051775602</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>6</v>
+        <v>1968.75</v>
       </c>
       <c r="B8">
-        <v>1968.75</v>
-      </c>
-      <c r="C8">
         <v>4.7283532484367896</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>7</v>
+        <v>1969</v>
       </c>
       <c r="B9">
-        <v>1969</v>
-      </c>
-      <c r="C9">
         <v>4.5625069075881699</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>8</v>
+        <v>1969.25</v>
       </c>
       <c r="B10">
-        <v>1969.25</v>
-      </c>
-      <c r="C10">
         <v>4.8161710635896</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>9</v>
+        <v>1969.5</v>
       </c>
       <c r="B11">
-        <v>1969.5</v>
-      </c>
-      <c r="C11">
         <v>4.7381865179139098</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>10</v>
+        <v>1969.75</v>
       </c>
       <c r="B12">
-        <v>1969.75</v>
-      </c>
-      <c r="C12">
         <v>4.9561278011516601</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>11</v>
+        <v>1970</v>
       </c>
       <c r="B13">
-        <v>1970</v>
-      </c>
-      <c r="C13">
         <v>3.6320163624337098</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>12</v>
+        <v>1970.25</v>
       </c>
       <c r="B14">
-        <v>1970.25</v>
-      </c>
-      <c r="C14">
         <v>2.6912294633031699</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>13</v>
+        <v>1970.5</v>
       </c>
       <c r="B15">
-        <v>1970.5</v>
-      </c>
-      <c r="C15">
         <v>2.0139921291421499</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>14</v>
+        <v>1970.75</v>
       </c>
       <c r="B16">
-        <v>1970.75</v>
-      </c>
-      <c r="C16">
         <v>0.67489930257233999</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>15</v>
+        <v>1971</v>
       </c>
       <c r="B17">
-        <v>1971</v>
-      </c>
-      <c r="C17">
         <v>1.5182257736871601</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>16</v>
+        <v>1971.25</v>
       </c>
       <c r="B18">
-        <v>1971.25</v>
-      </c>
-      <c r="C18">
         <v>1.5605981600486001</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>17</v>
+        <v>1971.5</v>
       </c>
       <c r="B19">
-        <v>1971.5</v>
-      </c>
-      <c r="C19">
         <v>1.01589798491457</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>18</v>
+        <v>1971.75</v>
       </c>
       <c r="B20">
-        <v>1971.75</v>
-      </c>
-      <c r="C20">
         <v>0.97591273937462897</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>19</v>
+        <v>1972</v>
       </c>
       <c r="B21">
-        <v>1972</v>
-      </c>
-      <c r="C21">
         <v>0.96944375906284896</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>20</v>
+        <v>1972.25</v>
       </c>
       <c r="B22">
-        <v>1972.25</v>
-      </c>
-      <c r="C22">
         <v>1.25369019092254</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>21</v>
+        <v>1972.5</v>
       </c>
       <c r="B23">
-        <v>1972.5</v>
-      </c>
-      <c r="C23">
         <v>1.1571177173289999</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>22</v>
+        <v>1972.75</v>
       </c>
       <c r="B24">
-        <v>1972.75</v>
-      </c>
-      <c r="C24">
         <v>1.5677526746778101</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>23</v>
+        <v>1973</v>
       </c>
       <c r="B25">
-        <v>1973</v>
-      </c>
-      <c r="C25">
         <v>3.0189354651204199</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>24</v>
+        <v>1973.25</v>
       </c>
       <c r="B26">
-        <v>1973.25</v>
-      </c>
-      <c r="C26">
         <v>3.4006461664701502</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>25</v>
+        <v>1973.5</v>
       </c>
       <c r="B27">
-        <v>1973.5</v>
-      </c>
-      <c r="C27">
         <v>3.3555989001693201</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>26</v>
+        <v>1973.75</v>
       </c>
       <c r="B28">
-        <v>1973.75</v>
-      </c>
-      <c r="C28">
         <v>3.2750078591151399</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>27</v>
+        <v>1974</v>
       </c>
       <c r="B29">
-        <v>1974</v>
-      </c>
-      <c r="C29">
         <v>2.69969465134354</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>28</v>
+        <v>1974.25</v>
       </c>
       <c r="B30">
-        <v>1974.25</v>
-      </c>
-      <c r="C30">
         <v>2.4770241864704801</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>29</v>
+        <v>1974.5</v>
       </c>
       <c r="B31">
-        <v>1974.5</v>
-      </c>
-      <c r="C31">
         <v>1.88966125065737</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>30</v>
+        <v>1974.75</v>
       </c>
       <c r="B32">
-        <v>1974.75</v>
-      </c>
-      <c r="C32">
         <v>6.8311422782629796E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>31</v>
+        <v>1975</v>
       </c>
       <c r="B33">
-        <v>1975</v>
-      </c>
-      <c r="C33">
         <v>-2.9064096154585899</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>32</v>
+        <v>1975.25</v>
       </c>
       <c r="B34">
-        <v>1975.25</v>
-      </c>
-      <c r="C34">
         <v>-3.9352288789090499</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>33</v>
+        <v>1975.5</v>
       </c>
       <c r="B35">
-        <v>1975.5</v>
-      </c>
-      <c r="C35">
         <v>-3.4686056527668399</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>34</v>
+        <v>1975.75</v>
       </c>
       <c r="B36">
-        <v>1975.75</v>
-      </c>
-      <c r="C36">
         <v>-2.9557038037216201</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>35</v>
+        <v>1976</v>
       </c>
       <c r="B37">
-        <v>1976</v>
-      </c>
-      <c r="C37">
         <v>-2.4026012081856898</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>36</v>
+        <v>1976.25</v>
       </c>
       <c r="B38">
-        <v>1976.25</v>
-      </c>
-      <c r="C38">
         <v>-1.9936172973028701</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>37</v>
+        <v>1976.5</v>
       </c>
       <c r="B39">
-        <v>1976.5</v>
-      </c>
-      <c r="C39">
         <v>-2.4132514008579098</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>38</v>
+        <v>1976.75</v>
       </c>
       <c r="B40">
-        <v>1976.75</v>
-      </c>
-      <c r="C40">
         <v>-2.6596875728361602</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>39</v>
+        <v>1977</v>
       </c>
       <c r="B41">
-        <v>1977</v>
-      </c>
-      <c r="C41">
         <v>-2.6664225666895298</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>40</v>
+        <v>1977.25</v>
       </c>
       <c r="B42">
-        <v>1977.25</v>
-      </c>
-      <c r="C42">
         <v>-2.0015745395454099</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>41</v>
+        <v>1977.5</v>
       </c>
       <c r="B43">
-        <v>1977.5</v>
-      </c>
-      <c r="C43">
         <v>-1.5229363699876799</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>42</v>
+        <v>1977.75</v>
       </c>
       <c r="B44">
-        <v>1977.75</v>
-      </c>
-      <c r="C44">
         <v>-0.924680641736364</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>43</v>
+        <v>1978</v>
       </c>
       <c r="B45">
-        <v>1978</v>
-      </c>
-      <c r="C45">
         <v>-0.73287709263073397</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>44</v>
+        <v>1978.25</v>
       </c>
       <c r="B46">
-        <v>1978.25</v>
-      </c>
-      <c r="C46">
         <v>-3.8379357578999201E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>45</v>
+        <v>1978.5</v>
       </c>
       <c r="B47">
-        <v>1978.5</v>
-      </c>
-      <c r="C47">
         <v>0.22336011412045201</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>46</v>
+        <v>1978.75</v>
       </c>
       <c r="B48">
-        <v>1978.75</v>
-      </c>
-      <c r="C48">
         <v>0.49768231277376102</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>47</v>
+        <v>1979</v>
       </c>
       <c r="B49">
-        <v>1979</v>
-      </c>
-      <c r="C49">
         <v>0.20473156482878599</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>48</v>
+        <v>1979.25</v>
       </c>
       <c r="B50">
-        <v>1979.25</v>
-      </c>
-      <c r="C50">
         <v>0.27505186548202298</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>49</v>
+        <v>1979.5</v>
       </c>
       <c r="B51">
-        <v>1979.5</v>
-      </c>
-      <c r="C51">
         <v>0.249984392217528</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>50</v>
+        <v>1979.75</v>
       </c>
       <c r="B52">
-        <v>1979.75</v>
-      </c>
-      <c r="C52">
         <v>-0.12884351334178001</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>51</v>
+        <v>1980</v>
       </c>
       <c r="B53">
-        <v>1980</v>
-      </c>
-      <c r="C53">
         <v>-0.66408845792400495</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>52</v>
+        <v>1980.25</v>
       </c>
       <c r="B54">
-        <v>1980.25</v>
-      </c>
-      <c r="C54">
         <v>-2.6856129030929199</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>53</v>
+        <v>1980.5</v>
       </c>
       <c r="B55">
-        <v>1980.5</v>
-      </c>
-      <c r="C55">
         <v>-3.9078726907999402</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>54</v>
+        <v>1980.75</v>
       </c>
       <c r="B56">
-        <v>1980.75</v>
-      </c>
-      <c r="C56">
         <v>-2.7041204818636002</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>55</v>
+        <v>1981</v>
       </c>
       <c r="B57">
-        <v>1981</v>
-      </c>
-      <c r="C57">
         <v>-2.1835412120195898</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>56</v>
+        <v>1981.25</v>
       </c>
       <c r="B58">
-        <v>1981.25</v>
-      </c>
-      <c r="C58">
         <v>-2.7332194963146299</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>57</v>
+        <v>1981.5</v>
       </c>
       <c r="B59">
-        <v>1981.5</v>
-      </c>
-      <c r="C59">
         <v>-2.6153856694562698</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>58</v>
+        <v>1981.75</v>
       </c>
       <c r="B60">
-        <v>1981.75</v>
-      </c>
-      <c r="C60">
         <v>-3.7280584492712601</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>59</v>
+        <v>1982</v>
       </c>
       <c r="B61">
-        <v>1982</v>
-      </c>
-      <c r="C61">
         <v>-4.5970227534724302</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>60</v>
+        <v>1982.25</v>
       </c>
       <c r="B62">
-        <v>1982.25</v>
-      </c>
-      <c r="C62">
         <v>-5.1006974384943202</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>61</v>
+        <v>1982.5</v>
       </c>
       <c r="B63">
-        <v>1982.5</v>
-      </c>
-      <c r="C63">
         <v>-6.1577650646407598</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>62</v>
+        <v>1982.75</v>
       </c>
       <c r="B64">
-        <v>1982.75</v>
-      </c>
-      <c r="C64">
         <v>-7.0304554974207703</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>63</v>
+        <v>1983</v>
       </c>
       <c r="B65">
-        <v>1983</v>
-      </c>
-      <c r="C65">
         <v>-5.9647924014370401</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>64</v>
+        <v>1983.25</v>
       </c>
       <c r="B66">
-        <v>1983.25</v>
-      </c>
-      <c r="C66">
         <v>-6.2955487391306901</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>65</v>
+        <v>1983.5</v>
       </c>
       <c r="B67">
-        <v>1983.5</v>
-      </c>
-      <c r="C67">
         <v>-5.2021467125123699</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>66</v>
+        <v>1983.75</v>
       </c>
       <c r="B68">
-        <v>1983.75</v>
-      </c>
-      <c r="C68">
         <v>-3.8156582184027599</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>67</v>
+        <v>1984</v>
       </c>
       <c r="B69">
-        <v>1984</v>
-      </c>
-      <c r="C69">
         <v>-3.42644201612775</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>68</v>
+        <v>1984.25</v>
       </c>
       <c r="B70">
-        <v>1984.25</v>
-      </c>
-      <c r="C70">
         <v>-2.9883749813335299</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>69</v>
+        <v>1984.5</v>
       </c>
       <c r="B71">
-        <v>1984.5</v>
-      </c>
-      <c r="C71">
         <v>-3.4868138293514401</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>70</v>
+        <v>1984.75</v>
       </c>
       <c r="B72">
-        <v>1984.75</v>
-      </c>
-      <c r="C72">
         <v>-2.99988939541905</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>71</v>
+        <v>1985</v>
       </c>
       <c r="B73">
-        <v>1985</v>
-      </c>
-      <c r="C73">
         <v>-2.6069623518107701</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>72</v>
+        <v>1985.25</v>
       </c>
       <c r="B74">
-        <v>1985.25</v>
-      </c>
-      <c r="C74">
         <v>-2.7142459529705398</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>73</v>
+        <v>1985.5</v>
       </c>
       <c r="B75">
-        <v>1985.5</v>
-      </c>
-      <c r="C75">
         <v>-2.4315938991020301</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>74</v>
+        <v>1985.75</v>
       </c>
       <c r="B76">
-        <v>1985.75</v>
-      </c>
-      <c r="C76">
         <v>-2.3214678835881002</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>75</v>
+        <v>1986</v>
       </c>
       <c r="B77">
-        <v>1986</v>
-      </c>
-      <c r="C77">
         <v>-2.2971131074700502</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>76</v>
+        <v>1986.25</v>
       </c>
       <c r="B78">
-        <v>1986.25</v>
-      </c>
-      <c r="C78">
         <v>-2.4291440187464199</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>77</v>
+        <v>1986.5</v>
       </c>
       <c r="B79">
-        <v>1986.5</v>
-      </c>
-      <c r="C79">
         <v>-2.39959038122548</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>78</v>
+        <v>1986.75</v>
       </c>
       <c r="B80">
-        <v>1986.75</v>
-      </c>
-      <c r="C80">
         <v>-2.0973830876962398</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>79</v>
+        <v>1987</v>
       </c>
       <c r="B81">
-        <v>1987</v>
-      </c>
-      <c r="C81">
         <v>-1.28674765235546</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>80</v>
+        <v>1987.25</v>
       </c>
       <c r="B82">
-        <v>1987.25</v>
-      </c>
-      <c r="C82">
         <v>-0.74007507514403104</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>81</v>
+        <v>1987.5</v>
       </c>
       <c r="B83">
-        <v>1987.5</v>
-      </c>
-      <c r="C83">
         <v>-0.29719638377579899</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>82</v>
+        <v>1987.75</v>
       </c>
       <c r="B84">
-        <v>1987.75</v>
-      </c>
-      <c r="C84">
         <v>0.39413841038386999</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>83</v>
+        <v>1988</v>
       </c>
       <c r="B85">
-        <v>1988</v>
-      </c>
-      <c r="C85">
         <v>9.9861070260298598E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>84</v>
+        <v>1988.25</v>
       </c>
       <c r="B86">
-        <v>1988.25</v>
-      </c>
-      <c r="C86">
         <v>0.29122093015720901</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>85</v>
+        <v>1988.5</v>
       </c>
       <c r="B87">
-        <v>1988.5</v>
-      </c>
-      <c r="C87">
         <v>0.10035339818748</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>86</v>
+        <v>1988.75</v>
       </c>
       <c r="B88">
-        <v>1988.75</v>
-      </c>
-      <c r="C88">
         <v>0.55683768681500301</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>87</v>
+        <v>1989</v>
       </c>
       <c r="B89">
-        <v>1989</v>
-      </c>
-      <c r="C89">
         <v>0.56185035472850997</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>88</v>
+        <v>1989.25</v>
       </c>
       <c r="B90">
-        <v>1989.25</v>
-      </c>
-      <c r="C90">
         <v>0.38443880240563999</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>89</v>
+        <v>1989.5</v>
       </c>
       <c r="B91">
-        <v>1989.5</v>
-      </c>
-      <c r="C91">
         <v>-2.2426477785664201E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>90</v>
+        <v>1989.75</v>
       </c>
       <c r="B92">
-        <v>1989.75</v>
-      </c>
-      <c r="C92">
         <v>-0.35224234576670599</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>91</v>
+        <v>1990</v>
       </c>
       <c r="B93">
-        <v>1990</v>
-      </c>
-      <c r="C93">
         <v>-0.29197120584721897</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>92</v>
+        <v>1990.25</v>
       </c>
       <c r="B94">
-        <v>1990.25</v>
-      </c>
-      <c r="C94">
         <v>-9.8732603861562102E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>93</v>
+        <v>1990.5</v>
       </c>
       <c r="B95">
-        <v>1990.5</v>
-      </c>
-      <c r="C95">
         <v>0.308654730960711</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>94</v>
+        <v>1990.75</v>
       </c>
       <c r="B96">
-        <v>1990.75</v>
-      </c>
-      <c r="C96">
         <v>-1.49721904285637E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>95</v>
+        <v>1991</v>
       </c>
       <c r="B97">
-        <v>1991</v>
-      </c>
-      <c r="C97">
         <v>-1.1890886816477599</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>96</v>
+        <v>1991.25</v>
       </c>
       <c r="B98">
-        <v>1991.25</v>
-      </c>
-      <c r="C98">
         <v>-1.42850661780156</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>97</v>
+        <v>1991.5</v>
       </c>
       <c r="B99">
-        <v>1991.5</v>
-      </c>
-      <c r="C99">
         <v>-1.03822494759203</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>98</v>
+        <v>1991.75</v>
       </c>
       <c r="B100">
-        <v>1991.75</v>
-      </c>
-      <c r="C100">
         <v>-0.69792383059062901</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>99</v>
+        <v>1992</v>
       </c>
       <c r="B101">
-        <v>1992</v>
-      </c>
-      <c r="C101">
         <v>-0.71978661027026702</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>100</v>
+        <v>1992.25</v>
       </c>
       <c r="B102">
-        <v>1992.25</v>
-      </c>
-      <c r="C102">
         <v>-0.99552107841550597</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>101</v>
+        <v>1992.5</v>
       </c>
       <c r="B103">
-        <v>1992.5</v>
-      </c>
-      <c r="C103">
         <v>-0.66674173292984296</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>102</v>
+        <v>1992.75</v>
       </c>
       <c r="B104">
-        <v>1992.75</v>
-      </c>
-      <c r="C104">
         <v>-0.56026303858947002</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>103</v>
+        <v>1993</v>
       </c>
       <c r="B105">
-        <v>1993</v>
-      </c>
-      <c r="C105">
         <v>6.3431958676529704E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>104</v>
+        <v>1993.25</v>
       </c>
       <c r="B106">
-        <v>1993.25</v>
-      </c>
-      <c r="C106">
         <v>0.13267604112141501</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>105</v>
+        <v>1993.5</v>
       </c>
       <c r="B107">
-        <v>1993.5</v>
-      </c>
-      <c r="C107">
         <v>0.62221956881969298</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>106</v>
+        <v>1993.75</v>
       </c>
       <c r="B108">
-        <v>1993.75</v>
-      </c>
-      <c r="C108">
         <v>0.26008176476561801</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>107</v>
+        <v>1994</v>
       </c>
       <c r="B109">
-        <v>1994</v>
-      </c>
-      <c r="C109">
         <v>-0.43509913798710498</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110">
-        <v>108</v>
+        <v>1994.25</v>
       </c>
       <c r="B110">
-        <v>1994.25</v>
-      </c>
-      <c r="C110">
         <v>-9.8659502897757698E-2</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111">
-        <v>109</v>
+        <v>1994.5</v>
       </c>
       <c r="B111">
-        <v>1994.5</v>
-      </c>
-      <c r="C111">
         <v>0.22132501897811299</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>110</v>
+        <v>1994.75</v>
       </c>
       <c r="B112">
-        <v>1994.75</v>
-      </c>
-      <c r="C112">
         <v>0.33422122010442401</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113">
-        <v>111</v>
+        <v>1995</v>
       </c>
       <c r="B113">
-        <v>1995</v>
-      </c>
-      <c r="C113">
         <v>0.52826703761092997</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114">
-        <v>112</v>
+        <v>1995.25</v>
       </c>
       <c r="B114">
-        <v>1995.25</v>
-      </c>
-      <c r="C114">
         <v>-4.46182668543793E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115">
-        <v>113</v>
+        <v>1995.5</v>
       </c>
       <c r="B115">
-        <v>1995.5</v>
-      </c>
-      <c r="C115">
         <v>-0.35994338475754301</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116">
-        <v>114</v>
+        <v>1995.75</v>
       </c>
       <c r="B116">
-        <v>1995.75</v>
-      </c>
-      <c r="C116">
         <v>-0.24151921803409099</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117">
-        <v>115</v>
+        <v>1996</v>
       </c>
       <c r="B117">
-        <v>1996</v>
-      </c>
-      <c r="C117">
         <v>-0.33266113352588</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118">
-        <v>116</v>
+        <v>1996.25</v>
       </c>
       <c r="B118">
-        <v>1996.25</v>
-      </c>
-      <c r="C118">
         <v>-9.0413553561985396E-2</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119">
-        <v>117</v>
+        <v>1996.5</v>
       </c>
       <c r="B119">
-        <v>1996.5</v>
-      </c>
-      <c r="C119">
         <v>0.182381904510275</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120">
-        <v>118</v>
+        <v>1996.75</v>
       </c>
       <c r="B120">
-        <v>1996.75</v>
-      </c>
-      <c r="C120">
         <v>-4.2084531755826E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121">
-        <v>119</v>
+        <v>1997</v>
       </c>
       <c r="B121">
-        <v>1997</v>
-      </c>
-      <c r="C121">
         <v>2.13653885948961E-2</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122">
-        <v>120</v>
+        <v>1997.25</v>
       </c>
       <c r="B122">
-        <v>1997.25</v>
-      </c>
-      <c r="C122">
         <v>-5.5512003547253299E-3</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123">
-        <v>121</v>
+        <v>1997.5</v>
       </c>
       <c r="B123">
-        <v>1997.5</v>
-      </c>
-      <c r="C123">
         <v>-0.17179571604927199</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124">
-        <v>122</v>
+        <v>1997.75</v>
       </c>
       <c r="B124">
-        <v>1997.75</v>
-      </c>
-      <c r="C124">
         <v>0.14700842385870699</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125">
-        <v>123</v>
+        <v>1998</v>
       </c>
       <c r="B125">
-        <v>1998</v>
-      </c>
-      <c r="C125">
         <v>-3.6127117898632197E-2</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126">
-        <v>124</v>
+        <v>1998.25</v>
       </c>
       <c r="B126">
-        <v>1998.25</v>
-      </c>
-      <c r="C126">
         <v>6.6443778686764404E-2</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127">
-        <v>125</v>
+        <v>1998.5</v>
       </c>
       <c r="B127">
-        <v>1998.5</v>
-      </c>
-      <c r="C127">
         <v>0.19929281405825999</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128">
-        <v>126</v>
+        <v>1998.75</v>
       </c>
       <c r="B128">
-        <v>1998.75</v>
-      </c>
-      <c r="C128">
         <v>0.144522464980023</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129">
-        <v>127</v>
+        <v>1999</v>
       </c>
       <c r="B129">
-        <v>1999</v>
-      </c>
-      <c r="C129">
         <v>0.22289788661582399</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130">
-        <v>128</v>
+        <v>1999.25</v>
       </c>
       <c r="B130">
-        <v>1999.25</v>
-      </c>
-      <c r="C130">
         <v>0.43197625799151701</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131">
-        <v>129</v>
+        <v>1999.5</v>
       </c>
       <c r="B131">
-        <v>1999.5</v>
-      </c>
-      <c r="C131">
         <v>0.77166750734176603</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132">
-        <v>130</v>
+        <v>1999.75</v>
       </c>
       <c r="B132">
-        <v>1999.75</v>
-      </c>
-      <c r="C132">
         <v>0.959921609063352</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133">
-        <v>131</v>
+        <v>2000</v>
       </c>
       <c r="B133">
-        <v>2000</v>
-      </c>
-      <c r="C133">
         <v>0.71871772044023097</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134">
-        <v>132</v>
+        <v>2000.25</v>
       </c>
       <c r="B134">
-        <v>2000.25</v>
-      </c>
-      <c r="C134">
         <v>1.0505716725935901</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135">
-        <v>133</v>
+        <v>2000.5</v>
       </c>
       <c r="B135">
-        <v>2000.5</v>
-      </c>
-      <c r="C135">
         <v>0.76640838485770801</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136">
-        <v>134</v>
+        <v>2000.75</v>
       </c>
       <c r="B136">
-        <v>2000.75</v>
-      </c>
-      <c r="C136">
         <v>0.649448105290795</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137">
-        <v>135</v>
+        <v>2001</v>
       </c>
       <c r="B137">
-        <v>2001</v>
-      </c>
-      <c r="C137">
         <v>0.75587526072544697</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138">
-        <v>136</v>
+        <v>2001.25</v>
       </c>
       <c r="B138">
-        <v>2001.25</v>
-      </c>
-      <c r="C138">
         <v>0.52826601641586801</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139">
-        <v>137</v>
+        <v>2001.5</v>
       </c>
       <c r="B139">
-        <v>2001.5</v>
-      </c>
-      <c r="C139">
         <v>0.64311443856388495</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140">
-        <v>138</v>
+        <v>2001.75</v>
       </c>
       <c r="B140">
-        <v>2001.75</v>
-      </c>
-      <c r="C140">
         <v>-0.26536005805783902</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141">
-        <v>139</v>
+        <v>2002</v>
       </c>
       <c r="B141">
-        <v>2002</v>
-      </c>
-      <c r="C141">
         <v>-0.832243771600227</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142">
-        <v>140</v>
+        <v>2002.25</v>
       </c>
       <c r="B142">
-        <v>2002.25</v>
-      </c>
-      <c r="C142">
         <v>-0.89289175654336805</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143">
-        <v>141</v>
+        <v>2002.5</v>
       </c>
       <c r="B143">
-        <v>2002.5</v>
-      </c>
-      <c r="C143">
         <v>-4.1484096016941502E-2</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144">
-        <v>142</v>
+        <v>2002.75</v>
       </c>
       <c r="B144">
-        <v>2002.75</v>
-      </c>
-      <c r="C144">
         <v>-3.5955928318032099E-2</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145">
-        <v>143</v>
+        <v>2003</v>
       </c>
       <c r="B145">
-        <v>2003</v>
-      </c>
-      <c r="C145">
         <v>0.288863317569654</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146">
-        <v>144</v>
+        <v>2003.25</v>
       </c>
       <c r="B146">
-        <v>2003.25</v>
-      </c>
-      <c r="C146">
         <v>-0.78563881232027699</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147">
-        <v>145</v>
+        <v>2003.5</v>
       </c>
       <c r="B147">
-        <v>2003.5</v>
-      </c>
-      <c r="C147">
         <v>-0.60393948013344101</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148">
-        <v>146</v>
+        <v>2003.75</v>
       </c>
       <c r="B148">
-        <v>2003.75</v>
-      </c>
-      <c r="C148">
         <v>3.1940206501834802E-2</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149">
-        <v>147</v>
+        <v>2004</v>
       </c>
       <c r="B149">
-        <v>2004</v>
-      </c>
-      <c r="C149">
         <v>7.1153323082984096E-2</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150">
-        <v>148</v>
+        <v>2004.25</v>
       </c>
       <c r="B150">
-        <v>2004.25</v>
-      </c>
-      <c r="C150">
         <v>0.64376876818388296</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151">
-        <v>149</v>
+        <v>2004.5</v>
       </c>
       <c r="B151">
-        <v>2004.5</v>
-      </c>
-      <c r="C151">
         <v>0.62309127434116895</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152">
-        <v>150</v>
+        <v>2004.75</v>
       </c>
       <c r="B152">
-        <v>2004.75</v>
-      </c>
-      <c r="C152">
         <v>0.68828875775868104</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153">
-        <v>151</v>
+        <v>2005</v>
       </c>
       <c r="B153">
-        <v>2005</v>
-      </c>
-      <c r="C153">
         <v>0.97464691962629801</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154">
-        <v>152</v>
+        <v>2005.25</v>
       </c>
       <c r="B154">
-        <v>2005.25</v>
-      </c>
-      <c r="C154">
         <v>0.90840817352761905</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155">
-        <v>153</v>
+        <v>2005.5</v>
       </c>
       <c r="B155">
-        <v>2005.5</v>
-      </c>
-      <c r="C155">
         <v>1.24972411553037</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156">
-        <v>154</v>
+        <v>2005.75</v>
       </c>
       <c r="B156">
-        <v>2005.75</v>
-      </c>
-      <c r="C156">
         <v>1.1326688940120599</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157">
-        <v>155</v>
+        <v>2006</v>
       </c>
       <c r="B157">
-        <v>2006</v>
-      </c>
-      <c r="C157">
         <v>1.5401235860984701</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158">
-        <v>156</v>
+        <v>2006.25</v>
       </c>
       <c r="B158">
-        <v>2006.25</v>
-      </c>
-      <c r="C158">
         <v>1.9053151153783401</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159">
-        <v>157</v>
+        <v>2006.5</v>
       </c>
       <c r="B159">
-        <v>2006.5</v>
-      </c>
-      <c r="C159">
         <v>1.6303302647433899</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160">
-        <v>158</v>
+        <v>2006.75</v>
       </c>
       <c r="B160">
-        <v>2006.75</v>
-      </c>
-      <c r="C160">
         <v>1.17679657090432</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161">
-        <v>159</v>
+        <v>2007</v>
       </c>
       <c r="B161">
-        <v>2007</v>
-      </c>
-      <c r="C161">
         <v>1.1004937282075</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162">
-        <v>160</v>
+        <v>2007.25</v>
       </c>
       <c r="B162">
-        <v>2007.25</v>
-      </c>
-      <c r="C162">
         <v>1.5370272094566699</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163">
-        <v>161</v>
+        <v>2007.5</v>
       </c>
       <c r="B163">
-        <v>2007.5</v>
-      </c>
-      <c r="C163">
         <v>1.64884679317744</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164">
-        <v>162</v>
+        <v>2007.75</v>
       </c>
       <c r="B164">
-        <v>2007.75</v>
-      </c>
-      <c r="C164">
         <v>1.7990681581704799</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165">
-        <v>163</v>
+        <v>2008</v>
       </c>
       <c r="B165">
-        <v>2008</v>
-      </c>
-      <c r="C165">
         <v>1.8991138331130299</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166">
-        <v>164</v>
+        <v>2008.25</v>
       </c>
       <c r="B166">
-        <v>2008.25</v>
-      </c>
-      <c r="C166">
         <v>2.4325786394589999</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167">
-        <v>165</v>
+        <v>2008.5</v>
       </c>
       <c r="B167">
-        <v>2008.5</v>
-      </c>
-      <c r="C167">
         <v>1.40517551076575</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168">
-        <v>166</v>
+        <v>2008.75</v>
       </c>
       <c r="B168">
-        <v>2008.75</v>
-      </c>
-      <c r="C168">
         <v>-0.96887400591048001</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169">
-        <v>167</v>
+        <v>2009</v>
       </c>
       <c r="B169">
-        <v>2009</v>
-      </c>
-      <c r="C169">
         <v>-2.9723186860581698</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170">
-        <v>168</v>
+        <v>2009.25</v>
       </c>
       <c r="B170">
-        <v>2009.25</v>
-      </c>
-      <c r="C170">
         <v>-4.1335786726438402</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171">
-        <v>169</v>
+        <v>2009.5</v>
       </c>
       <c r="B171">
-        <v>2009.5</v>
-      </c>
-      <c r="C171">
         <v>-3.7786272062196602</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172">
-        <v>170</v>
+        <v>2009.75</v>
       </c>
       <c r="B172">
-        <v>2009.75</v>
-      </c>
-      <c r="C172">
         <v>-3.4114255801871698</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173">
-        <v>171</v>
+        <v>2010</v>
       </c>
       <c r="B173">
-        <v>2010</v>
-      </c>
-      <c r="C173">
         <v>-3.4193878910709001</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174">
-        <v>172</v>
+        <v>2010.25</v>
       </c>
       <c r="B174">
-        <v>2010.25</v>
-      </c>
-      <c r="C174">
         <v>-2.8846679641841901</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175">
-        <v>173</v>
+        <v>2010.5</v>
       </c>
       <c r="B175">
-        <v>2010.5</v>
-      </c>
-      <c r="C175">
         <v>-2.5487002875683298</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176">
-        <v>174</v>
+        <v>2010.75</v>
       </c>
       <c r="B176">
-        <v>2010.75</v>
-      </c>
-      <c r="C176">
         <v>-2.4228777957718699</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177">
-        <v>175</v>
+        <v>2011</v>
       </c>
       <c r="B177">
-        <v>2011</v>
-      </c>
-      <c r="C177">
         <v>-1.85757438132121</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178">
-        <v>176</v>
+        <v>2011.25</v>
       </c>
       <c r="B178">
-        <v>2011.25</v>
-      </c>
-      <c r="C178">
         <v>-1.77917428761348</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179">
-        <v>177</v>
+        <v>2011.5</v>
       </c>
       <c r="B179">
-        <v>2011.5</v>
-      </c>
-      <c r="C179">
         <v>-1.1446424993198501</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180">
-        <v>178</v>
+        <v>2011.75</v>
       </c>
       <c r="B180">
-        <v>2011.75</v>
-      </c>
-      <c r="C180">
         <v>-1.09749933364705</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181">
-        <v>179</v>
+        <v>2012</v>
       </c>
       <c r="B181">
-        <v>2012</v>
-      </c>
-      <c r="C181">
         <v>-1.2296962482356999</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182">
-        <v>180</v>
+        <v>2012.25</v>
       </c>
       <c r="B182">
-        <v>2012.25</v>
-      </c>
-      <c r="C182">
         <v>-1.37190841025787</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183">
-        <v>181</v>
+        <v>2012.5</v>
       </c>
       <c r="B183">
-        <v>2012.5</v>
-      </c>
-      <c r="C183">
         <v>-1.4414173250124001</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184">
-        <v>182</v>
+        <v>2012.75</v>
       </c>
       <c r="B184">
-        <v>2012.75</v>
-      </c>
-      <c r="C184">
         <v>-1.26102124697407</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185">
-        <v>183</v>
+        <v>2013</v>
       </c>
       <c r="B185">
-        <v>2013</v>
-      </c>
-      <c r="C185">
         <v>-0.72331716815990899</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186">
-        <v>184</v>
+        <v>2013.25</v>
       </c>
       <c r="B186">
-        <v>2013.25</v>
-      </c>
-      <c r="C186">
         <v>-0.51096311740960099</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187">
-        <v>185</v>
+        <v>2013.5</v>
       </c>
       <c r="B187">
-        <v>2013.5</v>
-      </c>
-      <c r="C187">
         <v>8.4849172596057607E-2</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188">
-        <v>186</v>
+        <v>2013.75</v>
       </c>
       <c r="B188">
-        <v>2013.75</v>
-      </c>
-      <c r="C188">
         <v>0.75281003398153201</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189">
-        <v>187</v>
+        <v>2014</v>
       </c>
       <c r="B189">
-        <v>2014</v>
-      </c>
-      <c r="C189">
         <v>0.96362371162181903</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190">
-        <v>188</v>
+        <v>2014.25</v>
       </c>
       <c r="B190">
-        <v>2014.25</v>
-      </c>
-      <c r="C190">
         <v>1.62482396070684</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191">
-        <v>189</v>
+        <v>2014.5</v>
       </c>
       <c r="B191">
-        <v>2014.5</v>
-      </c>
-      <c r="C191">
         <v>1.93166827776307</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192">
-        <v>190</v>
+        <v>2014.75</v>
       </c>
       <c r="B192">
-        <v>2014.75</v>
-      </c>
-      <c r="C192">
         <v>1.6905671414536501</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193">
-        <v>191</v>
+        <v>2015</v>
       </c>
       <c r="B193">
-        <v>2015</v>
-      </c>
-      <c r="C193">
         <v>1.5464701542621599</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194">
-        <v>192</v>
+        <v>2015.25</v>
       </c>
       <c r="B194">
-        <v>2015.25</v>
-      </c>
-      <c r="C194">
         <v>1.6764965808915899</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195">
-        <v>193</v>
+        <v>2015.5</v>
       </c>
       <c r="B195">
-        <v>2015.5</v>
-      </c>
-      <c r="C195">
         <v>1.9706055700468399</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196">
-        <v>194</v>
+        <v>2015.75</v>
       </c>
       <c r="B196">
-        <v>2015.75</v>
-      </c>
-      <c r="C196">
         <v>1.79691817268348</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197">
-        <v>195</v>
+        <v>2016</v>
       </c>
       <c r="B197">
-        <v>2016</v>
-      </c>
-      <c r="C197">
         <v>1.8239827909722399</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198">
-        <v>196</v>
+        <v>2016.25</v>
       </c>
       <c r="B198">
-        <v>2016.25</v>
-      </c>
-      <c r="C198">
         <v>2.0218542414777301</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199">
-        <v>197</v>
+        <v>2016.5</v>
       </c>
       <c r="B199">
-        <v>2016.5</v>
-      </c>
-      <c r="C199">
         <v>2.45076147498912</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200">
-        <v>198</v>
+        <v>2016.75</v>
       </c>
       <c r="B200">
-        <v>2016.75</v>
-      </c>
-      <c r="C200">
         <v>2.4884442332342198</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201">
-        <v>199</v>
+        <v>2017</v>
       </c>
       <c r="B201">
-        <v>2017</v>
-      </c>
-      <c r="C201">
         <v>2.8170387253167299</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202">
-        <v>200</v>
+        <v>2017.25</v>
       </c>
       <c r="B202">
-        <v>2017.25</v>
-      </c>
-      <c r="C202">
         <v>3.0212935681556998</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203">
-        <v>201</v>
+        <v>2017.5</v>
       </c>
       <c r="B203">
-        <v>2017.5</v>
-      </c>
-      <c r="C203">
         <v>3.1473774841236102</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204">
-        <v>202</v>
+        <v>2017.75</v>
       </c>
       <c r="B204">
-        <v>2017.75</v>
-      </c>
-      <c r="C204">
         <v>3.0079972408547202</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205">
-        <v>203</v>
+        <v>2018</v>
       </c>
       <c r="B205">
-        <v>2018</v>
-      </c>
-      <c r="C205">
         <v>3.1953722024214302</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206">
-        <v>204</v>
+        <v>2018.25</v>
       </c>
       <c r="B206">
-        <v>2018.25</v>
-      </c>
-      <c r="C206">
         <v>3.3182716983495699</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207">
-        <v>205</v>
+        <v>2018.5</v>
       </c>
       <c r="B207">
-        <v>2018.5</v>
-      </c>
-      <c r="C207">
         <v>3.6166157306626499</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208">
-        <v>206</v>
+        <v>2018.75</v>
       </c>
       <c r="B208">
-        <v>2018.75</v>
-      </c>
-      <c r="C208">
         <v>3.4894803411561899</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209">
-        <v>207</v>
+        <v>2019</v>
       </c>
       <c r="B209">
-        <v>2019</v>
-      </c>
-      <c r="C209">
         <v>3.4712747999565199</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210">
-        <v>208</v>
+        <v>2019.25</v>
       </c>
       <c r="B210">
-        <v>2019.25</v>
-      </c>
-      <c r="C210">
         <v>3.5102662391488701</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211">
-        <v>209</v>
+        <v>2019.5</v>
       </c>
       <c r="B211">
-        <v>2019.5</v>
-      </c>
-      <c r="C211">
         <v>3.9494136447191601</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212">
-        <v>210</v>
+        <v>2019.75</v>
       </c>
       <c r="B212">
-        <v>2019.75</v>
-      </c>
-      <c r="C212">
         <v>3.68717340764357</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213">
-        <v>211</v>
+        <v>2020</v>
       </c>
       <c r="B213">
-        <v>2020</v>
-      </c>
-      <c r="C213">
         <v>1.6761107608405901</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214">
-        <v>212</v>
+        <v>2020.25</v>
       </c>
       <c r="B214">
-        <v>2020.25</v>
-      </c>
-      <c r="C214">
-        <v>-14.40282698</v>
+        <v>-14.24814379</v>
       </c>
     </row>
   </sheetData>

</xml_diff>